<commit_message>
enhance define_fast_field for query
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_tech/screenshots.xlsx
+++ b/lisha1.00/doc_tech/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23820" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25840" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -8993,20 +8993,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>697</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>719</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>730</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>754</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="152" name="Image 151"/>
+        <xdr:cNvPr id="159" name="Image 158"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9019,8 +9019,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2438400" y="132816600"/>
-          <a:ext cx="6692900" cy="4191000"/>
+          <a:off x="1485900" y="139065000"/>
+          <a:ext cx="6908800" cy="4737100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9039,19 +9039,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>721</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>727</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>755</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>774</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="153" name="Image 152"/>
+        <xdr:cNvPr id="160" name="Image 159"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -9064,8 +9064,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2971800" y="137439400"/>
-          <a:ext cx="10795000" cy="1155700"/>
+          <a:off x="2857500" y="143967200"/>
+          <a:ext cx="6731000" cy="3517900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9083,26 +9083,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>734</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>702</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>706</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>745</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="154" name="Rectangle 153"/>
+        <xdr:cNvPr id="161" name="Rectangle 160"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7086600" y="133756400"/>
-          <a:ext cx="1371600" cy="812800"/>
+          <a:off x="6019800" y="140004800"/>
+          <a:ext cx="1371600" cy="1968500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9155,26 +9155,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>707</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>712</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>744</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>745</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="155" name="Rectangle 154"/>
+        <xdr:cNvPr id="162" name="Rectangle 161"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7086600" y="134734300"/>
-          <a:ext cx="1371600" cy="952500"/>
+          <a:off x="2921000" y="141770100"/>
+          <a:ext cx="1397000" cy="203200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9227,26 +9227,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>653986</xdr:colOff>
-      <xdr:row>711</xdr:row>
-      <xdr:rowOff>174481</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>30142</xdr:colOff>
-      <xdr:row>725</xdr:row>
-      <xdr:rowOff>71726</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>392014</xdr:colOff>
+      <xdr:row>742</xdr:row>
+      <xdr:rowOff>190077</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>607884</xdr:colOff>
+      <xdr:row>772</xdr:row>
+      <xdr:rowOff>18610</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="156" name="Flèche vers la gauche 155"/>
+        <xdr:cNvPr id="163" name="Flèche vers la gauche 162"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="14711485">
-          <a:off x="7727691" y="136801276"/>
-          <a:ext cx="2564245" cy="201656"/>
+        <a:xfrm rot="14149359">
+          <a:off x="2681182" y="144204909"/>
+          <a:ext cx="5543533" cy="215870"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
@@ -9292,26 +9292,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>116212</xdr:colOff>
-      <xdr:row>705</xdr:row>
-      <xdr:rowOff>124766</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>339311</xdr:colOff>
-      <xdr:row>725</xdr:row>
-      <xdr:rowOff>134139</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>735746</xdr:colOff>
+      <xdr:row>745</xdr:row>
+      <xdr:rowOff>127690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>126421</xdr:colOff>
+      <xdr:row>762</xdr:row>
+      <xdr:rowOff>37613</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="157" name="Flèche vers la gauche 156"/>
+        <xdr:cNvPr id="164" name="Flèche vers la gauche 163"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm rot="14711485">
-          <a:off x="7398575" y="136225403"/>
-          <a:ext cx="3819373" cy="223099"/>
+        <a:xfrm rot="15779919">
+          <a:off x="5873622" y="143516314"/>
+          <a:ext cx="3148423" cy="216175"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
@@ -9358,25 +9358,97 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>724</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>726</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>769</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>770</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="158" name="Rectangle 157"/>
+        <xdr:cNvPr id="165" name="Rectangle 164"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6845300" y="138099800"/>
-          <a:ext cx="6781800" cy="279400"/>
+          <a:off x="7061200" y="146621500"/>
+          <a:ext cx="1955800" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>762</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>769</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="166" name="Rectangle 165"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7061200" y="145224500"/>
+          <a:ext cx="2057400" cy="1384300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9754,8 +9826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A693" workbookViewId="0">
-      <selection activeCell="O695" sqref="O695"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A742" workbookViewId="0">
+      <selection activeCell="M760" sqref="M760"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
operator ok and some doc enhancement But advanced filter not yet completed
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_tech/screenshots.xlsx
+++ b/lisha1.00/doc_tech/screenshots.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="16840" tabRatio="500"/>
@@ -9894,6 +9894,476 @@
           <a:ext cx="520700" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>815</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>825</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="153" name="Image 152"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1651000" y="155257500"/>
+          <a:ext cx="2794000" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>816</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>818</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="172" name="Ellipse 171"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2895600" y="155600400"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>816</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>823</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="155" name="Image 154"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791200" y="155625800"/>
+          <a:ext cx="2273300" cy="1270000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>818</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>819</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="173" name="Ellipse 172"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6756400" y="155879800"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dashDot"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>831</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>839</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="156" name="Image 155"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476500" y="158305500"/>
+          <a:ext cx="2565400" cy="1612900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>832</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>834</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="174" name="Ellipse 173"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4025900" y="158661100"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dashDot"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>833</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>840</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="157" name="Image 156"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6616700" y="158711900"/>
+          <a:ext cx="1866900" cy="1333500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>834</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>836</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="175" name="Ellipse 174"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7607300" y="159004000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
@@ -10269,8 +10739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A781" workbookViewId="0">
-      <selection activeCell="L803" sqref="L803"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A810" workbookViewId="0">
+      <selection activeCell="K826" sqref="K826"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Global search enhancement and documentation updated
</commit_message>
<xml_diff>
--- a/lisha1.00/doc_tech/screenshots.xlsx
+++ b/lisha1.00/doc_tech/screenshots.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="16840" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="360" windowWidth="20160" windowHeight="16840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10370,6 +10374,241 @@
           <a:solidFill>
             <a:srgbClr val="FF0000"/>
           </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>846</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>850</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="158" name="Image 157"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="977900" y="161188400"/>
+          <a:ext cx="2146300" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>847</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>848</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="176" name="Ellipse 175"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952500" y="161366200"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="50800" dir="3780000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>845</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>850</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="177" name="Image 176"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5321300" y="161137600"/>
+          <a:ext cx="2197100" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>846</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>848</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="178" name="Ellipse 177"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5207000" y="161277300"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="dashDot"/>
           <a:tailEnd type="arrow"/>
         </a:ln>
         <a:effectLst>
@@ -10739,8 +10978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A810" workbookViewId="0">
-      <selection activeCell="K826" sqref="K826"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A826" workbookViewId="0">
+      <selection activeCell="H844" sqref="H844"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>